<commit_message>
update after session 1
</commit_message>
<xml_diff>
--- a/DataSets/PortlandHousingPrices.xlsx
+++ b/DataSets/PortlandHousingPrices.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1010" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="1940" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Num Bedrooms</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">Downloaded from </t>
   </si>
@@ -36,10 +33,19 @@
     <t>http://openclassroom.stanford.edu/MainFolder/DocumentPage.php?course=MachineLearning&amp;doc=exercises/ex3/ex3.html</t>
   </si>
   <si>
-    <t>Price ($)</t>
+    <t>Num Bedrooms(x1)</t>
   </si>
   <si>
-    <t>Area (Square Feet)</t>
+    <t>Area (Square Feet) (x2)</t>
+  </si>
+  <si>
+    <t>Price ($) - output or target</t>
+  </si>
+  <si>
+    <t>Prediction</t>
+  </si>
+  <si>
+    <t>COST</t>
   </si>
 </sst>
 </file>
@@ -384,10 +390,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -398,18 +405,21 @@
     <col min="4" max="4" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>3</v>
       </c>
@@ -420,7 +430,7 @@
         <v>399900</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -431,7 +441,7 @@
         <v>329900</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -442,7 +452,7 @@
         <v>369000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -453,7 +463,7 @@
         <v>232000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -464,7 +474,7 @@
         <v>539900</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -475,7 +485,7 @@
         <v>299900</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -486,7 +496,7 @@
         <v>314900</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -497,7 +507,7 @@
         <v>198999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>3</v>
       </c>
@@ -508,7 +518,7 @@
         <v>212000</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -519,7 +529,7 @@
         <v>242500</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>4</v>
       </c>
@@ -530,7 +540,7 @@
         <v>239999</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>3</v>
       </c>
@@ -541,7 +551,7 @@
         <v>347000</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>3</v>
       </c>
@@ -552,7 +562,7 @@
         <v>329999</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>5</v>
       </c>
@@ -563,7 +573,7 @@
         <v>699900</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -924,6 +934,11 @@
       </c>
       <c r="C48" s="3">
         <v>239500</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C49" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -943,12 +958,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned housing prices file
</commit_message>
<xml_diff>
--- a/DataSets/PortlandHousingPrices.xlsx
+++ b/DataSets/PortlandHousingPrices.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="2870" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">Downloaded from </t>
   </si>
@@ -40,12 +40,6 @@
   </si>
   <si>
     <t>Price ($) - output or target</t>
-  </si>
-  <si>
-    <t>Prediction</t>
-  </si>
-  <si>
-    <t>COST</t>
   </si>
 </sst>
 </file>
@@ -390,11 +384,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="116" zoomScaleNormal="116" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -415,9 +409,7 @@
       <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
@@ -934,11 +926,6 @@
       </c>
       <c r="C48" s="3">
         <v>239500</v>
-      </c>
-    </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
-      <c r="C49" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>